<commit_message>
weight decay 1e-5 version
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis_miRNA/Downregulated Genes Analyzed/mouse_go_analysis_results_miRNA_downregulated.xlsx
+++ b/gene_ontology_analysis_miRNA/Downregulated Genes Analyzed/mouse_go_analysis_results_miRNA_downregulated.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/gene_ontology_analysis_miRNA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/gene_ontology_analysis_miRNA/Downregulated Genes Analyzed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3124AD84-1265-BB4B-8D55-7449BCA496B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672EF18C-BF96-6C4D-88D1-AB263D49B6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11560" yWindow="500" windowWidth="37540" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11560" yWindow="500" windowWidth="37540" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biological Process" sheetId="1" r:id="rId1"/>
     <sheet name="Molecular Function" sheetId="2" r:id="rId2"/>
     <sheet name="Cellular Component" sheetId="3" r:id="rId3"/>
+    <sheet name="Final Table Downregulated" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="742">
   <si>
     <t>Rank</t>
   </si>
@@ -2228,13 +2229,79 @@
   </si>
   <si>
     <t>FAM171A1</t>
+  </si>
+  <si>
+    <t>Functional Category</t>
+  </si>
+  <si>
+    <t>Key Processes (Biological/Molecular/Cellular Combined)</t>
+  </si>
+  <si>
+    <t>Significance</t>
+  </si>
+  <si>
+    <t>Neuron projection morphogenesis, synapse assembly, filopodium assembly, synaptic vesicle recycling</t>
+  </si>
+  <si>
+    <t>NLGN1, GPM6A, TBC1D24, KLF7, FLRT1</t>
+  </si>
+  <si>
+    <t>Very High (p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>Negative regulation of cytokine production, inflammatory response, interferon production</t>
+  </si>
+  <si>
+    <t>NLRC3, BCL6, MACIR, GNL1</t>
+  </si>
+  <si>
+    <t>High (p&lt;0.005)</t>
+  </si>
+  <si>
+    <t>Membrane &amp; Cell Junction Organization</t>
+  </si>
+  <si>
+    <t>Cell junction assembly, plasma membrane organization, filopodium assembly</t>
+  </si>
+  <si>
+    <t>Cholesterol transport, efflux, storage, homeostasis</t>
+  </si>
+  <si>
+    <t>Moderate (p&lt;0.05)</t>
+  </si>
+  <si>
+    <t>DNA damage response, MAPK cascade, NF-kappaB signaling</t>
+  </si>
+  <si>
+    <t>MAP3K20, PHLPP1, MDM4, JCAD</t>
+  </si>
+  <si>
+    <t>Transcription termination, RNA polymerase activity</t>
+  </si>
+  <si>
+    <t>Protein Modification</t>
+  </si>
+  <si>
+    <t>Protein glycosylation, ubiquitination</t>
+  </si>
+  <si>
+    <t>UBE2E3, TUSC3, DOLPP1</t>
+  </si>
+  <si>
+    <t>Cell Projection Organization</t>
+  </si>
+  <si>
+    <t>Plasma membrane bounded cell projection, cilium assembly</t>
+  </si>
+  <si>
+    <t>TBC1D24, TBC1D8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2246,18 +2313,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2294,7 +2355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2310,6 +2371,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2347,10 +2420,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2359,20 +2429,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2677,10 +2752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P408"/>
+  <dimension ref="A1:O408"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2698,7 +2773,7 @@
     <col min="15" max="15" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2727,7 +2802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2756,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2785,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2814,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2843,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2872,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2901,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2930,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2959,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2987,21 +3062,20 @@
       <c r="I10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="5" t="s">
         <v>642</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="P10" s="7"/>
-    </row>
-    <row r="11" spans="1:16" ht="80" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3029,21 +3103,20 @@
       <c r="I11" s="2">
         <v>0</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="6" t="s">
         <v>645</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="P11" s="7"/>
-    </row>
-    <row r="12" spans="1:16" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3071,21 +3144,20 @@
       <c r="I12" s="2">
         <v>0</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>647</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="O12" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="P12" s="7"/>
-    </row>
-    <row r="13" spans="1:16" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3113,21 +3185,20 @@
       <c r="I13" s="2">
         <v>0</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="8" t="s">
         <v>649</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="4" t="s">
         <v>650</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="P13" s="7"/>
-    </row>
-    <row r="14" spans="1:16" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3155,21 +3226,20 @@
       <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="N14" s="6" t="s">
         <v>653</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="P14" s="7"/>
-    </row>
-    <row r="15" spans="1:16" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3197,21 +3267,20 @@
       <c r="I15" s="2">
         <v>0</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="N15" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="P15" s="7"/>
-    </row>
-    <row r="16" spans="1:16" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3239,21 +3308,20 @@
       <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="8" t="s">
         <v>657</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="4" t="s">
         <v>658</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N16" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="O16" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="P16" s="7"/>
-    </row>
-    <row r="17" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3281,21 +3349,20 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="8" t="s">
         <v>660</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="N17" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="O17" s="5" t="s">
+      <c r="O17" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3327,7 +3394,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3359,7 +3426,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3391,7 +3458,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3423,7 +3490,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3455,7 +3522,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3487,7 +3554,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3519,7 +3586,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3551,7 +3618,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3583,7 +3650,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3615,7 +3682,7 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3647,7 +3714,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3679,7 +3746,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3711,7 +3778,7 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3743,7 +3810,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -15125,16 +15192,16 @@
       <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="M14" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="N14" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="O14" s="12" t="s">
+      <c r="O14" s="9" t="s">
         <v>642</v>
       </c>
-      <c r="P14" s="12" t="s">
+      <c r="P14" s="9" t="s">
         <v>661</v>
       </c>
     </row>
@@ -15166,16 +15233,16 @@
       <c r="I15" s="2">
         <v>0</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="M15" s="8" t="s">
         <v>671</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="O15" s="6" t="s">
         <v>645</v>
       </c>
-      <c r="P15" s="10" t="s">
+      <c r="P15" s="4" t="s">
         <v>690</v>
       </c>
     </row>
@@ -15207,16 +15274,16 @@
       <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="8" t="s">
         <v>672</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="P16" s="4" t="s">
         <v>663</v>
       </c>
     </row>
@@ -15248,16 +15315,16 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="8" t="s">
         <v>674</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="4" t="s">
         <v>675</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="O17" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="P17" s="4" t="s">
         <v>691</v>
       </c>
     </row>
@@ -15289,16 +15356,16 @@
       <c r="I18" s="2">
         <v>0</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="8" t="s">
         <v>676</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="O18" s="6" t="s">
         <v>653</v>
       </c>
-      <c r="P18" s="10" t="s">
+      <c r="P18" s="4" t="s">
         <v>692</v>
       </c>
     </row>
@@ -15330,16 +15397,16 @@
       <c r="I19" s="2">
         <v>0</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="8" t="s">
         <v>678</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="O19" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="P19" s="4" t="s">
         <v>693</v>
       </c>
     </row>
@@ -15371,16 +15438,16 @@
       <c r="I20" s="2">
         <v>0</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="8" t="s">
         <v>680</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="O20" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="P20" s="10" t="s">
+      <c r="P20" s="4" t="s">
         <v>694</v>
       </c>
     </row>
@@ -15412,16 +15479,16 @@
       <c r="I21" s="2">
         <v>0</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="8" t="s">
         <v>682</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="P21" s="10" t="s">
+      <c r="P21" s="4" t="s">
         <v>695</v>
       </c>
     </row>
@@ -15453,16 +15520,16 @@
       <c r="I22" s="2">
         <v>0</v>
       </c>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="8" t="s">
         <v>684</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="O22" s="6" t="s">
         <v>686</v>
       </c>
-      <c r="P22" s="10" t="s">
+      <c r="P22" s="4" t="s">
         <v>696</v>
       </c>
     </row>
@@ -15494,16 +15561,16 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="8" t="s">
         <v>688</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="O23" s="8" t="s">
+      <c r="O23" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="P23" s="10" t="s">
+      <c r="P23" s="4" t="s">
         <v>697</v>
       </c>
     </row>
@@ -15538,7 +15605,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="9"/>
+      <c r="P24" s="7"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
@@ -15571,7 +15638,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="9"/>
+      <c r="P25" s="7"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
@@ -15604,7 +15671,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="9"/>
+      <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -15637,7 +15704,7 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="9"/>
+      <c r="P27" s="7"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -15670,7 +15737,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="9"/>
+      <c r="P28" s="7"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -15703,7 +15770,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="9"/>
+      <c r="P29" s="7"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
@@ -15736,7 +15803,7 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="9"/>
+      <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -15769,7 +15836,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
-      <c r="P31" s="9"/>
+      <c r="P31" s="7"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
@@ -15802,7 +15869,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="9"/>
+      <c r="P32" s="7"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -15835,7 +15902,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="9"/>
+      <c r="P33" s="7"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -15868,7 +15935,7 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
-      <c r="P34" s="9"/>
+      <c r="P34" s="7"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
@@ -15901,7 +15968,7 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
-      <c r="P35" s="9"/>
+      <c r="P35" s="7"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -15934,7 +16001,7 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
-      <c r="P36" s="9"/>
+      <c r="P36" s="7"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -15967,7 +16034,7 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-      <c r="P37" s="9"/>
+      <c r="P37" s="7"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
@@ -16000,7 +16067,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-      <c r="P38" s="9"/>
+      <c r="P38" s="7"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
@@ -16033,7 +16100,7 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-      <c r="P39" s="9"/>
+      <c r="P39" s="7"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
@@ -16066,7 +16133,7 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="9"/>
+      <c r="P40" s="7"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
@@ -16099,7 +16166,7 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="9"/>
+      <c r="P41" s="7"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -16132,7 +16199,7 @@
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
-      <c r="P42" s="9"/>
+      <c r="P42" s="7"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
@@ -16165,7 +16232,7 @@
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
-      <c r="P43" s="9"/>
+      <c r="P43" s="7"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
@@ -16195,10 +16262,10 @@
       <c r="I44" s="2">
         <v>0</v>
       </c>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -16228,10 +16295,10 @@
       <c r="I45" s="2">
         <v>0</v>
       </c>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -16261,10 +16328,10 @@
       <c r="I46" s="2">
         <v>0</v>
       </c>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -16294,10 +16361,10 @@
       <c r="I47" s="2">
         <v>0</v>
       </c>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -16327,10 +16394,10 @@
       <c r="I48" s="2">
         <v>0</v>
       </c>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -16360,10 +16427,10 @@
       <c r="I49" s="2">
         <v>0</v>
       </c>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
@@ -16393,10 +16460,10 @@
       <c r="I50" s="2">
         <v>0</v>
       </c>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
@@ -16426,10 +16493,10 @@
       <c r="I51" s="2">
         <v>0</v>
       </c>
-      <c r="M51" s="9"/>
-      <c r="N51" s="9"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
@@ -16459,10 +16526,10 @@
       <c r="I52" s="2">
         <v>0</v>
       </c>
-      <c r="M52" s="9"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
@@ -16492,10 +16559,10 @@
       <c r="I53" s="2">
         <v>0</v>
       </c>
-      <c r="M53" s="9"/>
-      <c r="N53" s="9"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
@@ -17290,7 +17357,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17946,16 +18013,16 @@
       <c r="I22" s="2">
         <v>0</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="L22" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="M22" s="9" t="s">
         <v>642</v>
       </c>
-      <c r="N22" s="12" t="s">
+      <c r="N22" s="9" t="s">
         <v>661</v>
       </c>
     </row>
@@ -17987,16 +18054,16 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="8" t="s">
         <v>699</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="M23" s="8" t="s">
+      <c r="M23" s="6" t="s">
         <v>645</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="4" t="s">
         <v>701</v>
       </c>
     </row>
@@ -18028,16 +18095,16 @@
       <c r="I24" s="2">
         <v>0</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="8" t="s">
         <v>702</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="4" t="s">
         <v>704</v>
       </c>
     </row>
@@ -18069,16 +18136,16 @@
       <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="4" t="s">
         <v>707</v>
       </c>
     </row>
@@ -18110,16 +18177,16 @@
       <c r="I26" s="2">
         <v>0</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="8" t="s">
         <v>708</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="M26" s="8" t="s">
+      <c r="M26" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="4" t="s">
         <v>710</v>
       </c>
     </row>
@@ -18151,16 +18218,16 @@
       <c r="I27" s="2">
         <v>0</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="L27" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="N27" s="4" t="s">
         <v>713</v>
       </c>
     </row>
@@ -18192,16 +18259,16 @@
       <c r="I28" s="2">
         <v>0</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="K28" s="8" t="s">
         <v>714</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="L28" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="M28" s="8" t="s">
+      <c r="M28" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" s="4" t="s">
         <v>716</v>
       </c>
     </row>
@@ -18233,16 +18300,16 @@
       <c r="I29" s="2">
         <v>0</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="8" t="s">
         <v>717</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="4" t="s">
         <v>718</v>
       </c>
-      <c r="M29" s="8" t="s">
+      <c r="M29" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" s="4" t="s">
         <v>719</v>
       </c>
     </row>
@@ -18992,4 +19059,347 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97B4F72-2537-B64C-B3CC-0FA562C76B2C}">
+  <dimension ref="D7:G48"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D7" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="D8" s="12" t="s">
+        <v>643</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>723</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>724</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="D9" s="12" t="s">
+        <v>646</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>726</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="D10" s="12" t="s">
+        <v>729</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>730</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>668</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="D11" s="12" t="s">
+        <v>651</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>663</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="D12" s="12" t="s">
+        <v>654</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>733</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>734</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="D13" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>735</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>665</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="D14" s="12" t="s">
+        <v>736</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>737</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>738</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="D15" s="12" t="s">
+        <v>739</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>740</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>741</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finalize miRNA best/worst corel gene tables
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis_miRNA/Downregulated Genes Analyzed/mouse_go_analysis_results_miRNA_downregulated.xlsx
+++ b/gene_ontology_analysis_miRNA/Downregulated Genes Analyzed/mouse_go_analysis_results_miRNA_downregulated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/gene_ontology_analysis_miRNA/Downregulated Genes Analyzed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26493C65-81CF-214E-BA9A-9D5D911669C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105DA45D-4A75-B548-A050-1BF4167C5DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13660" yWindow="500" windowWidth="37540" windowHeight="26600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="2080" windowWidth="37540" windowHeight="26600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biological Process" sheetId="1" r:id="rId1"/>
@@ -2781,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O408"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A362" workbookViewId="0">
-      <selection activeCell="A403" sqref="A403:G403"/>
+    <sheetView showGridLines="0" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14811,8 +14811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:G78"/>
+    <sheetView showGridLines="0" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17399,8 +17399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:G38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>